<commit_message>
Listo informe semanal 220812
</commit_message>
<xml_diff>
--- a/tabla.xlsx
+++ b/tabla.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja5" sheetId="5" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
-    <sheet name="TECO2" sheetId="2" r:id="rId3"/>
-    <sheet name="CEPU" sheetId="3" r:id="rId4"/>
-    <sheet name="BYMA" sheetId="6" r:id="rId5"/>
-    <sheet name="ARS=X" sheetId="4" r:id="rId6"/>
+    <sheet name="LOMA" sheetId="10" r:id="rId3"/>
+    <sheet name="TGSU2" sheetId="9" r:id="rId4"/>
+    <sheet name="PAMP" sheetId="8" r:id="rId5"/>
+    <sheet name="TECO2" sheetId="2" r:id="rId6"/>
+    <sheet name="CEPU" sheetId="3" r:id="rId7"/>
+    <sheet name="BYMA" sheetId="6" r:id="rId8"/>
+    <sheet name="ARS=X" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="98">
   <si>
     <t>TICKER</t>
   </si>
@@ -269,16 +272,71 @@
   </si>
   <si>
     <t>Resultado operativo</t>
+  </si>
+  <si>
+    <t>US$ M</t>
+  </si>
+  <si>
+    <t>QoQ</t>
+  </si>
+  <si>
+    <t>ND / EV</t>
+  </si>
+  <si>
+    <t>EV / EBITDA</t>
+  </si>
+  <si>
+    <t>EV / SALES</t>
+  </si>
+  <si>
+    <t>M ARS</t>
+  </si>
+  <si>
+    <t>M USD</t>
+  </si>
+  <si>
+    <t>Sales Natural Gas Trans.</t>
+  </si>
+  <si>
+    <t>Liquids producttion &amp; commer.</t>
+  </si>
+  <si>
+    <t>Other Services</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Ventas mercado domestico casi en su totalidad</t>
+  </si>
+  <si>
+    <t>EBITDA adj</t>
+  </si>
+  <si>
+    <t>Net Debt</t>
+  </si>
+  <si>
+    <t>Net Debt / EBITDA LTM adj</t>
+  </si>
+  <si>
+    <t>Otros Servicios</t>
+  </si>
+  <si>
+    <t>Prod. y Com. de Líquidos</t>
+  </si>
+  <si>
+    <t>Transp. de Gas Natural</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="0&quot; M&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -380,20 +438,20 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -414,6 +472,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -421,6 +481,15 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -440,22 +509,13 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0,,\ &quot; M&quot;"/>
+      <numFmt numFmtId="164" formatCode="#,##0,,\ &quot; M&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,6 +530,966 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6894-4E6A-AA74-6CA3172315A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6894-4E6A-AA74-6CA3172315A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6894-4E6A-AA74-6CA3172315A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3888888888888888E-2"/>
+                  <c:y val="4.6296296296296294E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-6894-4E6A-AA74-6CA3172315A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.8888779527559053E-2"/>
+                  <c:y val="-7.1759259259259411E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.23556933508311462"/>
+                      <c:h val="0.34733814523184592"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6894-4E6A-AA74-6CA3172315A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6666666666666666E-2"/>
+                  <c:y val="4.1666666666666664E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-6894-4E6A-AA74-6CA3172315A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>TGSU2!$L$2:$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Transp. de Gas Natural</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Prod. y Com. de Líquidos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Otros Servicios</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TGSU2!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>0" M"</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8241</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3626</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6894-4E6A-AA74-6CA3172315A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>747712</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:K4" totalsRowShown="0">
   <autoFilter ref="A1:K4"/>
@@ -482,12 +1502,12 @@
     <tableColumn id="6" name="EBIT" dataDxfId="4">
       <calculatedColumnFormula>E2-693000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="EBIT mg" dataDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="7" name="EBIT mg" dataDxfId="3" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Tabla1[[#This Row],[EBIT]]/Tabla1[[#This Row],[SALES]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NI" dataDxfId="3"/>
-    <tableColumn id="9" name="Deuda Neta" dataDxfId="2"/>
-    <tableColumn id="10" name="MC" dataDxfId="1"/>
+    <tableColumn id="8" name="NI" dataDxfId="2"/>
+    <tableColumn id="9" name="Deuda Neta" dataDxfId="1"/>
+    <tableColumn id="10" name="MC" dataDxfId="0"/>
     <tableColumn id="11" name="DN / EV" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>Tabla1[Deuda Neta]/(Tabla1[MC]+Tabla1[Deuda Neta])</calculatedColumnFormula>
     </tableColumn>
@@ -774,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
@@ -1527,6 +2547,1116 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>147</v>
+      </c>
+      <c r="C2">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2/B2-1</f>
+        <v>0.38775510204081631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3/B3-1</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B3/B2</f>
+        <v>0.32653061224489793</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C3/C2</f>
+        <v>0.30882352941176472</v>
+      </c>
+      <c r="D5" s="11">
+        <f>(C5-B5)*100</f>
+        <v>-1.7707082833133214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7/B7-1</f>
+        <v>0.12244897959183665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <f>C9/B9-1</f>
+        <v>-0.95348837209302328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10">
+        <v>0.12</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>305000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>207993100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20">
+        <f>B19+B18</f>
+        <v>208298100000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="31">
+        <f>B18/B20</f>
+        <v>1.4642476335597877E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="str">
+        <f>B1</f>
+        <v>2T21</v>
+      </c>
+      <c r="H1" t="str">
+        <f t="shared" ref="H1:I1" si="0">C1</f>
+        <v>2T22</v>
+      </c>
+      <c r="I1" t="str">
+        <f t="shared" si="0"/>
+        <v>YoY</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>8357</v>
+      </c>
+      <c r="C2">
+        <v>8241</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D4" si="1">C2/B2-1</f>
+        <v>-1.3880579155199246E-2</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F4" si="2">A2</f>
+        <v>Sales Natural Gas Trans.</v>
+      </c>
+      <c r="G2" s="26">
+        <f ca="1">B2/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>88.976914435414642</v>
+      </c>
+      <c r="H2" s="26">
+        <f ca="1">C2/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>67.812900943305877</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I4" ca="1" si="3">H2/G2-1</f>
+        <v>-0.23785960241935578</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="32">
+        <f>C2</f>
+        <v>8241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>18246</v>
+      </c>
+      <c r="C3">
+        <v>16206</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.11180532719500169</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="2"/>
+        <v>Liquids producttion &amp; commer.</v>
+      </c>
+      <c r="G3" s="26">
+        <f ca="1">B3/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>194.26502103488997</v>
+      </c>
+      <c r="H3" s="26">
+        <f ca="1">C3/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>133.35467451610424</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.31354253171416913</v>
+      </c>
+      <c r="L3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="32">
+        <f t="shared" ref="M3:M4" si="4">C3</f>
+        <v>16206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
+        <v>2759</v>
+      </c>
+      <c r="C4">
+        <v>3626</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31424429140993104</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>Other Services</v>
+      </c>
+      <c r="G4" s="26">
+        <f ca="1">B4/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>29.375051684493119</v>
+      </c>
+      <c r="H4" s="26">
+        <f ca="1">C4/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>29.837347266160307</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.5737694239061684E-2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M4" s="32">
+        <f t="shared" si="4"/>
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>29362</v>
+      </c>
+      <c r="C5">
+        <v>28073</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5/B5-1</f>
+        <v>-4.3900279272529152E-2</v>
+      </c>
+      <c r="F5" t="str">
+        <f>A5</f>
+        <v>VENTAS</v>
+      </c>
+      <c r="G5" s="26">
+        <f ca="1">B5/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>312.61698715479776</v>
+      </c>
+      <c r="H5" s="26">
+        <f ca="1">C5/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>231.0049227255704</v>
+      </c>
+      <c r="I5" s="1">
+        <f ca="1">H5/G5-1</f>
+        <v>-0.26106087571247594</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>13447</v>
+      </c>
+      <c r="C6">
+        <v>12697</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6/B6-1</f>
+        <v>-5.5774522198259846E-2</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F10" si="5">A6</f>
+        <v>EBITDA</v>
+      </c>
+      <c r="G6" s="26">
+        <f ca="1">B6/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>143.17010511104709</v>
+      </c>
+      <c r="H6" s="26">
+        <f ca="1">C6/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>104.48008776570254</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I7" ca="1" si="6">H6/G6-1</f>
+        <v>-0.27023810114084501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>10191</v>
+      </c>
+      <c r="C7">
+        <v>9327</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7/B7-1</f>
+        <v>-8.4780688843096863E-2</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="5"/>
+        <v>EBIT</v>
+      </c>
+      <c r="G7" s="26">
+        <f ca="1">B7/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>108.50349826628103</v>
+      </c>
+      <c r="H7" s="26">
+        <f ca="1">C7/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>76.749293422911521</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.29265604658608102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B6/B5</f>
+        <v>0.45797289013010012</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C6/C5</f>
+        <v>0.4522851138104228</v>
+      </c>
+      <c r="D8" s="11">
+        <f>(C8-B8)*100</f>
+        <v>-0.56877763196773179</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="5"/>
+        <v>EBITDA mg</v>
+      </c>
+      <c r="G8" s="3">
+        <f>B8</f>
+        <v>0.45797289013010012</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8:H9" si="7">C8</f>
+        <v>0.4522851138104228</v>
+      </c>
+      <c r="I8" s="11">
+        <f>(H8-G8)*100</f>
+        <v>-0.56877763196773179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B7/B5</f>
+        <v>0.34708126149444862</v>
+      </c>
+      <c r="C9" s="1">
+        <f>C7/C5</f>
+        <v>0.33224094325508496</v>
+      </c>
+      <c r="D9" s="11">
+        <f>(C9-B9)*100</f>
+        <v>-1.4840318239363659</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="5"/>
+        <v>EBIT mg</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9" si="8">B9</f>
+        <v>0.34708126149444862</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.33224094325508496</v>
+      </c>
+      <c r="I9" s="11">
+        <f>(H9-G9)*100</f>
+        <v>-1.4840318239363659</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="e">
+        <f>C10/B10-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="5"/>
+        <v>NI</v>
+      </c>
+      <c r="G10">
+        <f ca="1">B10/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f ca="1">C10/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" ref="I10" ca="1" si="9">H10/G10-1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" t="str">
+        <f>B12</f>
+        <v>2T21</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" ref="H12" si="10">C12</f>
+        <v>2T22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>70050</v>
+      </c>
+      <c r="C13">
+        <v>64438</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F15" si="11">A13</f>
+        <v>LT debt</v>
+      </c>
+      <c r="G13" s="26">
+        <f ca="1">B13/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>732.69077659668301</v>
+      </c>
+      <c r="H13" s="26">
+        <f ca="1">C13/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>479.98510242085661</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="11"/>
+        <v>LT leasings</v>
+      </c>
+      <c r="G14" s="26">
+        <f ca="1">B14/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="26">
+        <f ca="1">C14/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>1609</v>
+      </c>
+      <c r="C15">
+        <v>1457</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="11"/>
+        <v>ST debt</v>
+      </c>
+      <c r="G15" s="26">
+        <f ca="1">B15/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>16.829399850736088</v>
+      </c>
+      <c r="H15" s="26">
+        <f ca="1">C15/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>10.852886405959032</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
+        <f>A16</f>
+        <v>ST leasings</v>
+      </c>
+      <c r="G16" s="26">
+        <f ca="1">B16/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="26">
+        <f ca="1">C16/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B13:B16)</f>
+        <v>71659</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C13:C16)</f>
+        <v>65895</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" ref="F17:F20" si="12">A17</f>
+        <v>DEBT</v>
+      </c>
+      <c r="G17" s="26">
+        <f ca="1">B17/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>749.52017644741909</v>
+      </c>
+      <c r="H17" s="26">
+        <f ca="1">C17/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>490.83798882681566</v>
+      </c>
+      <c r="I17" s="1">
+        <f ca="1">H17/G17-1</f>
+        <v>-0.3451303857445267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>6036</v>
+      </c>
+      <c r="C18">
+        <v>4233</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="12"/>
+        <v>Caja y eq</v>
+      </c>
+      <c r="G18" s="26">
+        <f ca="1">B18/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>63.133783405247378</v>
+      </c>
+      <c r="H18" s="26">
+        <f ca="1">C18/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>31.53072625698324</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <f>18083+30592</f>
+        <v>48675</v>
+      </c>
+      <c r="C19">
+        <f>21188+27973</f>
+        <v>49161</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="12"/>
+        <v>Inversiones ST</v>
+      </c>
+      <c r="G19" s="26">
+        <f ca="1">B19/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>509.11810921975086</v>
+      </c>
+      <c r="H19" s="26">
+        <f ca="1">C19/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>366.18994413407819</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <f>B17-SUM(B18:B19)</f>
+        <v>16948</v>
+      </c>
+      <c r="C20">
+        <f>C17-SUM(C18:C19)</f>
+        <v>12501</v>
+      </c>
+      <c r="D20" s="1">
+        <f>C20/B20-1</f>
+        <v>-0.26239084257729528</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="12"/>
+        <v>NET DEBT</v>
+      </c>
+      <c r="G20" s="26">
+        <f ca="1">B20/VLOOKUP(G$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>177.2682838224209</v>
+      </c>
+      <c r="H20" s="26">
+        <f ca="1">C20/VLOOKUP(H$1,Tabla2[[#All],[Q]:[Ave.]],2,0)</f>
+        <v>93.117318435754186</v>
+      </c>
+      <c r="I20" s="1">
+        <f ca="1">H20/G20-1</f>
+        <v>-0.47470965235363383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>285221200000</v>
+      </c>
+      <c r="C23">
+        <f>B23/1000000</f>
+        <v>285221.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <f>C20*1000000</f>
+        <v>12501000000</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:C25" si="13">B24/1000000</f>
+        <v>12501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <f>B23+B24</f>
+        <v>297722200000</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="13"/>
+        <v>297722.2</v>
+      </c>
+      <c r="F25">
+        <f ca="1">2632/'ARS=X'!G8</f>
+        <v>21.657997243390493</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="1">
+        <f>B24/B25</f>
+        <v>4.1988807015398921E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28">
+        <f>B25/(C6*1000000)</f>
+        <v>23.448231865795069</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29">
+        <f>B25/(C5*1000000)</f>
+        <v>10.605286218074307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>346</v>
+      </c>
+      <c r="C2">
+        <f>874-462</f>
+        <v>412</v>
+      </c>
+      <c r="D2">
+        <v>462</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2/C2-1</f>
+        <v>0.12135922330097082</v>
+      </c>
+      <c r="F2" s="1">
+        <f>D2/B2-1</f>
+        <v>0.33526011560693636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>202</v>
+      </c>
+      <c r="C3">
+        <f>375-D3</f>
+        <v>183</v>
+      </c>
+      <c r="D3">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E4" si="0">D3/C3-1</f>
+        <v>4.9180327868852514E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>D3/B3-1</f>
+        <v>-4.9504950495049549E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>154</v>
+      </c>
+      <c r="C4">
+        <f>269-D4</f>
+        <v>133</v>
+      </c>
+      <c r="D4">
+        <v>136</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2556390977443552E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>D4/B4-1</f>
+        <v>-0.11688311688311692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B3/B2</f>
+        <v>0.58381502890173409</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:D5" si="1">C3/C2</f>
+        <v>0.44417475728155342</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.41558441558441561</v>
+      </c>
+      <c r="E5" s="11">
+        <f>(D5-C5)*100</f>
+        <v>-2.8590341697137811</v>
+      </c>
+      <c r="F5" s="11">
+        <f>(D5-B5)*100</f>
+        <v>-16.823061331731846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B4/B2</f>
+        <v>0.44508670520231214</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:D6" si="2">C4/C2</f>
+        <v>0.32281553398058255</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2943722943722944</v>
+      </c>
+      <c r="E6" s="11">
+        <f>(D6-C6)*100</f>
+        <v>-2.8443239608288149</v>
+      </c>
+      <c r="F6" s="11">
+        <f>(D6-B6)*100</f>
+        <v>-15.071441083001774</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <f>165-D7</f>
+        <v>99</v>
+      </c>
+      <c r="D7">
+        <v>66</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7" si="3">D7/C7-1</f>
+        <v>-0.33333333333333337</v>
+      </c>
+      <c r="F7" s="1">
+        <f>D7/B7-1</f>
+        <v>-5.7142857142857162E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>902</v>
+      </c>
+      <c r="F17">
+        <f>D17-B17</f>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>1327700000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <f>D17*1000000</f>
+        <v>902000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <f>B20+B21</f>
+        <v>2229700000</v>
+      </c>
+      <c r="C22">
+        <f>B22/1000000</f>
+        <v>2229.6999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23">
+        <f>B21/B22</f>
+        <v>0.40453872718302913</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25">
+        <f>B22/(D3*1000000)</f>
+        <v>11.613020833333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26">
+        <f>B22/(D2*1000000)</f>
+        <v>4.8261904761904759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1749,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -2331,7 +4461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2417,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G422"/>
   <sheetViews>

</xml_diff>